<commit_message>
Began Python program, excelstuff is obsolete
</commit_message>
<xml_diff>
--- a/excel/excelstuff.xlsx
+++ b/excel/excelstuff.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26207"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicco\PycharmProjects\Elmag-lab-4\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicco/PycharmProjects/Elmag-lab-4/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -126,13 +129,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,7 +204,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -209,7 +212,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -236,7 +239,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -260,7 +263,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="nb-NO"/>
   <c:roundedCorners val="0"/>
@@ -312,7 +315,7 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.255</c:v>
@@ -324,7 +327,7 @@
                   <c:v>0.754</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.25</c:v>
@@ -333,25 +336,25 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7490000000000001</c:v>
+                  <c:v>1.749</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.2519999999999998</c:v>
+                  <c:v>2.252</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.4990000000000001</c:v>
+                  <c:v>2.499</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.7490000000000001</c:v>
+                  <c:v>2.749</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.0009999999999999</c:v>
+                  <c:v>3.001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.2509999999999999</c:v>
+                  <c:v>3.251</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>3.504</c:v>
@@ -360,19 +363,19 @@
                   <c:v>3.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.9980000000000002</c:v>
+                  <c:v>3.998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.2510000000000003</c:v>
+                  <c:v>4.251</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.5049999999999999</c:v>
+                  <c:v>4.505</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.7489999999999997</c:v>
+                  <c:v>4.749</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.9989999999999997</c:v>
+                  <c:v>4.999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -384,16 +387,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.8E-2</c:v>
+                  <c:v>0.078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11600000000000001</c:v>
+                  <c:v>0.116</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.154</c:v>
@@ -402,22 +405,22 @@
                   <c:v>0.193</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23100000000000001</c:v>
+                  <c:v>0.231</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.26900000000000002</c:v>
+                  <c:v>0.269</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.308</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.34599999999999997</c:v>
+                  <c:v>0.346</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.38400000000000001</c:v>
+                  <c:v>0.384</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.42199999999999999</c:v>
+                  <c:v>0.422</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.46</c:v>
@@ -426,31 +429,31 @@
                   <c:v>0.499</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.53800000000000003</c:v>
+                  <c:v>0.538</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.57499999999999996</c:v>
+                  <c:v>0.575</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.61299999999999999</c:v>
+                  <c:v>0.613</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.65200000000000002</c:v>
+                  <c:v>0.652</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.69</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.72799999999999998</c:v>
+                  <c:v>0.728</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.76600000000000001</c:v>
+                  <c:v>0.766</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-425C-4A72-879D-AC429E2D071C}"/>
             </c:ext>
@@ -481,7 +484,7 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.255</c:v>
@@ -493,7 +496,7 @@
                   <c:v>0.754</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.25</c:v>
@@ -502,25 +505,25 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7490000000000001</c:v>
+                  <c:v>1.749</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.2519999999999998</c:v>
+                  <c:v>2.252</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.4990000000000001</c:v>
+                  <c:v>2.499</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.7490000000000001</c:v>
+                  <c:v>2.749</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.0009999999999999</c:v>
+                  <c:v>3.001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.2509999999999999</c:v>
+                  <c:v>3.251</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>3.504</c:v>
@@ -529,19 +532,19 @@
                   <c:v>3.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.9980000000000002</c:v>
+                  <c:v>3.998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.2510000000000003</c:v>
+                  <c:v>4.251</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.5049999999999999</c:v>
+                  <c:v>4.505</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.7489999999999997</c:v>
+                  <c:v>4.749</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.9989999999999997</c:v>
+                  <c:v>4.999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -553,73 +556,73 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>9.7738977907252931E-4</c:v>
+                  <c:v>0.000977389779072529</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0020364545986099E-2</c:v>
+                  <c:v>0.0400203645459861</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.8297790788058208E-2</c:v>
+                  <c:v>0.0782977907880582</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11642210732516205</c:v>
+                  <c:v>0.116422107325162</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15408709474736101</c:v>
+                  <c:v>0.154087094747361</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.19236452098943313</c:v>
+                  <c:v>0.192364520989433</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23064194723150527</c:v>
+                  <c:v>0.230641947231505</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.26876626376860913</c:v>
+                  <c:v>0.268766263768609</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.3071967997156495</c:v>
+                  <c:v>0.307196799715649</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.34578044536765817</c:v>
+                  <c:v>0.345780445367658</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.3835985424948255</c:v>
+                  <c:v>0.383598542494825</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.42187596873689759</c:v>
+                  <c:v>0.421875968736898</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.46045961438890626</c:v>
+                  <c:v>0.460459614388906</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.4987370406309784</c:v>
+                  <c:v>0.498737040630978</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.53747379598795542</c:v>
+                  <c:v>0.537473795987955</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.57513878341015445</c:v>
+                  <c:v>0.575138783410154</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.61310999024228996</c:v>
+                  <c:v>0.61310999024229</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.65184674559926703</c:v>
+                  <c:v>0.651846745599267</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.69073661066121217</c:v>
+                  <c:v>0.690736610661212</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.72809537867347451</c:v>
+                  <c:v>0.728095378673474</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.76637280491554671</c:v>
+                  <c:v>0.766372804915547</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-425C-4A72-879D-AC429E2D071C}"/>
             </c:ext>
@@ -633,11 +636,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="346428752"/>
-        <c:axId val="359505184"/>
+        <c:axId val="2096746432"/>
+        <c:axId val="2096750128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="346428752"/>
+        <c:axId val="2096746432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,12 +697,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359505184"/>
+        <c:crossAx val="2096750128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="359505184"/>
+        <c:axId val="2096750128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -756,7 +759,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346428752"/>
+        <c:crossAx val="2096746432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1381,7 +1384,7 @@
         <xdr:cNvPr id="3" name="Diagram 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD7891DE-B4F4-4EF6-BC64-5362EDE604E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AD7891DE-B4F4-4EF6-BC64-5362EDE604E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1701,31 +1704,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75">
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1753,7 +1756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16.5" thickBot="1">
+    <row r="7" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1765,7 +1768,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>0</v>
       </c>
@@ -1789,7 +1792,7 @@
         <v>-9.7738977907252931E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>0.255</v>
       </c>
@@ -1813,7 +1816,7 @@
         <v>-2.0364545986098492E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>0.505</v>
       </c>
@@ -1837,7 +1840,7 @@
         <v>-2.9779078805820813E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>0.754</v>
       </c>
@@ -1861,7 +1864,7 @@
         <v>-4.2210732516204108E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -1885,7 +1888,7 @@
         <v>-8.7094747361016189E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>1.25</v>
       </c>
@@ -1909,7 +1912,7 @@
         <v>6.3547901056687506E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>1.5</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>3.5805276849473766E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>1.7490000000000001</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>2.3373623139089084E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>2</v>
       </c>
@@ -1981,7 +1984,7 @@
         <v>8.0320028435049151E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>2.2519999999999998</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>2.1955463234180073E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>2.4990000000000001</v>
       </c>
@@ -2029,7 +2032,7 @@
         <v>4.0145750517450729E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>2.7490000000000001</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>1.2403126310239765E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>3.0009999999999999</v>
       </c>
@@ -2077,7 +2080,7 @@
         <v>-4.5961438890623763E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>3.2509999999999999</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>2.6295936902159811E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>3.504</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>5.2620401204461764E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>3.75</v>
       </c>
@@ -2149,7 +2152,7 @@
         <v>-1.3878341015449713E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>3.9980000000000002</v>
       </c>
@@ -2173,7 +2176,7 @@
         <v>-1.0999024228997012E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>4.2510000000000003</v>
       </c>
@@ -2197,7 +2200,7 @@
         <v>1.532544007329939E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>4.5049999999999999</v>
       </c>
@@ -2221,7 +2224,7 @@
         <v>-7.3661066121222252E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>4.7489999999999997</v>
       </c>
@@ -2245,7 +2248,7 @@
         <v>-9.5378673474533215E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
         <v>4.9989999999999997</v>
       </c>
@@ -2269,7 +2272,7 @@
         <v>-3.7280491554669837E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="10">
         <f>SUM(A8:A28)</f>
         <v>52.521000000000008</v>
@@ -2286,31 +2289,28 @@
         <f t="shared" si="4"/>
         <v>27.525663999999995</v>
       </c>
-      <c r="E29" s="11">
-        <f>SUM(E31:E51)</f>
-        <v>3.9895048780440557E-6</v>
-      </c>
+      <c r="E29" s="11"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E31">
-        <f>(B8-$A$34-$B$34*A8)^2</f>
+        <f t="shared" ref="E31:E51" si="5">(B8-$A$34-$B$34*A8)^2</f>
         <v>9.5529078023544763E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E32">
-        <f>(B9-$A$34-$B$34*A9)^2</f>
+        <f t="shared" si="5"/>
         <v>4.147147332199202E-10</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E33">
-        <f>(B10-$A$34-$B$34*A10)^2</f>
+        <f t="shared" si="5"/>
         <v>8.8679353452328636E-8</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <f>(C29*B29-A29*D29)/(COUNT(A8:A28)*C29-(A29^2))</f>
         <v>9.7738977907252931E-4</v>
@@ -2320,117 +2320,117 @@
         <v>0.15310970496828849</v>
       </c>
       <c r="E34">
-        <f>(B11-$A$34-$B$34*A11)^2</f>
+        <f t="shared" si="5"/>
         <v>1.7817459395545308E-7</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E35">
-        <f>(B12-$A$34-$B$34*A12)^2</f>
+        <f t="shared" si="5"/>
         <v>7.5854950178792364E-9</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E36">
-        <f>(B13-$A$34-$B$34*A13)^2</f>
+        <f t="shared" si="5"/>
         <v>4.0383357287105451E-7</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E37">
-        <f>(B14-$A$34-$B$34*A14)^2</f>
+        <f t="shared" si="5"/>
         <v>1.2820178502674619E-7</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E38">
-        <f>(B15-$A$34-$B$34*A15)^2</f>
+        <f t="shared" si="5"/>
         <v>5.463262586481606E-8</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E39">
-        <f>(B16-$A$34-$B$34*A16)^2</f>
+        <f t="shared" si="5"/>
         <v>6.4513069678071042E-7</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <f>SQRT((1/(COUNT(A8:A28)-2))*(E29*C29/(COUNT(A8:A28)*C29-(A29^2))))</f>
-        <v>1.9316166905250843E-4</v>
+        <v>0</v>
       </c>
       <c r="B40">
         <f>SQRT((COUNT(A8:A28)/(COUNT(A8:A28)-2))*(E29/(COUNT(A8:A28)*C29-(A29^2))))</f>
-        <v>6.60797509249102E-5</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <f>(B17-$A$34-$B$34*A17)^2</f>
+        <f t="shared" si="5"/>
         <v>4.8204236582743291E-8</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E41">
-        <f>(B18-$A$34-$B$34*A18)^2</f>
+        <f t="shared" si="5"/>
         <v>1.6116812846093955E-7</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E42">
-        <f>(B19-$A$34-$B$34*A19)^2</f>
+        <f t="shared" si="5"/>
         <v>1.5383754226776189E-8</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E43">
-        <f>(B20-$A$34-$B$34*A20)^2</f>
+        <f t="shared" si="5"/>
         <v>2.1124538648965424E-7</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E44">
-        <f>(B21-$A$34-$B$34*A21)^2</f>
+        <f t="shared" si="5"/>
         <v>6.9147629756237006E-8</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E45">
-        <f>(B22-$A$34-$B$34*A22)^2</f>
+        <f t="shared" si="5"/>
         <v>2.7689066229185209E-7</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E46">
-        <f>(B23-$A$34-$B$34*A23)^2</f>
+        <f t="shared" si="5"/>
         <v>1.9260834934111378E-8</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E47">
-        <f>(B24-$A$34-$B$34*A24)^2</f>
+        <f t="shared" si="5"/>
         <v>1.2097853399006331E-8</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E48">
-        <f>(B25-$A$34-$B$34*A25)^2</f>
+        <f t="shared" si="5"/>
         <v>2.3486911344029081E-8</v>
       </c>
     </row>
-    <row r="49" spans="5:5">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E49">
-        <f>(B26-$A$34-$B$34*A26)^2</f>
+        <f t="shared" si="5"/>
         <v>5.4259526621150771E-7</v>
       </c>
     </row>
-    <row r="50" spans="5:5">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E50">
-        <f>(B27-$A$34-$B$34*A27)^2</f>
+        <f t="shared" si="5"/>
         <v>9.0970913537616258E-9</v>
       </c>
     </row>
-    <row r="51" spans="5:5">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E51">
-        <f>(B28-$A$34-$B$34*A28)^2</f>
+        <f t="shared" si="5"/>
         <v>1.389835050557809E-7</v>
       </c>
     </row>

</xml_diff>